<commit_message>
Refactor CSV comparator to interlace columns and highlight differences
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,32 +452,27 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Name_file2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Age_file1</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Age_file2</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Location_file1</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Name_file2</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Age_file2</t>
-        </is>
-      </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Location_file2</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>extra col_file2</t>
         </is>
       </c>
     </row>
@@ -490,29 +485,26 @@
           <t>John</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
         <v>30</v>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="n">
+        <v>30</v>
+      </c>
+      <c r="F2" t="inlineStr">
         <is>
           <t xml:space="preserve">New York </t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>John</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>30</v>
-      </c>
       <c r="G2" t="inlineStr">
         <is>
           <t>New York</t>
         </is>
-      </c>
-      <c r="H2" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -524,29 +516,26 @@
           <t>Susan</t>
         </is>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Susan</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="F3" t="inlineStr">
         <is>
           <t>Los Angeles</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Susan</t>
-        </is>
-      </c>
-      <c r="F3" s="2" t="n">
-        <v>26</v>
-      </c>
       <c r="G3" t="inlineStr">
         <is>
           <t>Los Angeles</t>
         </is>
-      </c>
-      <c r="H3" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -558,29 +547,26 @@
           <t>David</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>David</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
         <v>35</v>
       </c>
-      <c r="D4" s="2" t="inlineStr">
+      <c r="E4" t="n">
+        <v>35</v>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
         <is>
           <t>Chicago</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>David</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>35</v>
-      </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
           <t>Houston</t>
         </is>
-      </c>
-      <c r="H4" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -592,41 +578,37 @@
           <t>Emily</t>
         </is>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C5" s="2" t="inlineStr"/>
+      <c r="D5" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="D5" s="2" t="inlineStr">
+      <c r="E5" s="2" t="inlineStr"/>
+      <c r="F5" s="2" t="inlineStr">
         <is>
           <t>Miami</t>
         </is>
       </c>
-      <c r="E5" s="2" t="inlineStr"/>
-      <c r="F5" s="2" t="inlineStr"/>
       <c r="G5" s="2" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="inlineStr"/>
-      <c r="C6" s="2" t="inlineStr"/>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>Michael</t>
+        </is>
+      </c>
       <c r="D6" s="2" t="inlineStr"/>
-      <c r="E6" s="2" t="inlineStr">
-        <is>
-          <t>Michael</t>
-        </is>
-      </c>
-      <c r="F6" s="2" t="n">
+      <c r="E6" s="2" t="n">
         <v>32</v>
       </c>
+      <c r="F6" s="2" t="inlineStr"/>
       <c r="G6" s="2" t="inlineStr">
         <is>
           <t>San Francisco</t>
         </is>
-      </c>
-      <c r="H6" t="n">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor CSV comparator code to include merge indicator and row status
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,170 +442,200 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Name_file1</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Name_file2</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Age_file1</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Age_file2</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Location_file1</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Location_file2</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>matched</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>John</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>John</t>
         </is>
-      </c>
-      <c r="D2" t="n">
-        <v>30</v>
       </c>
       <c r="E2" t="n">
         <v>30</v>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" t="n">
+        <v>30</v>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t xml:space="preserve">New York </t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>New York</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>not matched</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>Susan</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>Susan</t>
         </is>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="E3" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="F3" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>Los Angeles</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>Los Angeles</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>not matched</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>3</v>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>David</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>David</t>
         </is>
-      </c>
-      <c r="D4" t="n">
-        <v>35</v>
       </c>
       <c r="E4" t="n">
         <v>35</v>
       </c>
-      <c r="F4" s="2" t="inlineStr">
+      <c r="F4" t="n">
+        <v>35</v>
+      </c>
+      <c r="G4" s="2" t="inlineStr">
         <is>
           <t>Chicago</t>
         </is>
       </c>
-      <c r="G4" s="2" t="inlineStr">
+      <c r="H4" s="2" t="inlineStr">
         <is>
           <t>Houston</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="inlineStr">
+      <c r="C5" s="2" t="inlineStr">
         <is>
           <t>Emily</t>
         </is>
       </c>
-      <c r="C5" s="2" t="inlineStr"/>
-      <c r="D5" s="2" t="n">
+      <c r="D5" s="2" t="inlineStr"/>
+      <c r="E5" s="2" t="n">
         <v>28</v>
       </c>
-      <c r="E5" s="2" t="inlineStr"/>
-      <c r="F5" s="2" t="inlineStr">
+      <c r="F5" s="2" t="inlineStr"/>
+      <c r="G5" s="2" t="inlineStr">
         <is>
           <t>Miami</t>
         </is>
       </c>
-      <c r="G5" s="2" t="inlineStr"/>
+      <c r="H5" s="2" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>missing</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="inlineStr"/>
-      <c r="C6" s="2" t="inlineStr">
+      <c r="C6" s="2" t="inlineStr"/>
+      <c r="D6" s="2" t="inlineStr">
         <is>
           <t>Michael</t>
         </is>
       </c>
-      <c r="D6" s="2" t="inlineStr"/>
-      <c r="E6" s="2" t="n">
+      <c r="E6" s="2" t="inlineStr"/>
+      <c r="F6" s="2" t="n">
         <v>32</v>
       </c>
-      <c r="F6" s="2" t="inlineStr"/>
-      <c r="G6" s="2" t="inlineStr">
+      <c r="G6" s="2" t="inlineStr"/>
+      <c r="H6" s="2" t="inlineStr">
         <is>
           <t>San Francisco</t>
         </is>

</xml_diff>